<commit_message>
Improved Check Validity Visual
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-1 (26 Juli 2021 - 29 Agustus 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-1 (26 Juli 2021 - 29 Agustus 2021).xlsx
@@ -1646,7 +1646,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="Z6" s="57" t="inlineStr"/>
+      <c r="Z6" s="50" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="AA6" s="49" t="inlineStr">
         <is>
           <t>ü</t>
@@ -5015,7 +5019,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="AF29" s="57" t="inlineStr"/>
+      <c r="AF29" s="50" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="AG29" s="45" t="inlineStr"/>
     </row>
     <row r="30" ht="15.6" customHeight="1">

</xml_diff>

<commit_message>
Smaller Image Size When Viewing
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-1 (26 Juli 2021 - 29 Agustus 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-1 (26 Juli 2021 - 29 Agustus 2021).xlsx
@@ -2709,7 +2709,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="S13" s="48" t="inlineStr"/>
+      <c r="S13" s="55" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="T13" s="54" t="inlineStr">
         <is>
           <t>ü</t>
@@ -2727,7 +2731,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="Y13" s="49" t="inlineStr"/>
+      <c r="Y13" s="56" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="Z13" s="51" t="inlineStr">
         <is>
           <t>ü</t>
@@ -2746,7 +2754,11 @@
         </is>
       </c>
       <c r="AE13" s="46" t="inlineStr"/>
-      <c r="AF13" s="59" t="inlineStr"/>
+      <c r="AF13" s="51" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="AG13" s="46" t="inlineStr"/>
     </row>
     <row r="14" ht="15.6" customHeight="1" s="1">
@@ -5501,7 +5513,11 @@
         </is>
       </c>
       <c r="X31" s="58" t="inlineStr"/>
-      <c r="Y31" s="49" t="inlineStr"/>
+      <c r="Y31" s="56" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="Z31" s="51" t="inlineStr">
         <is>
           <t>ü</t>

</xml_diff>

<commit_message>
Merge Bug Fixed & File Update
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-1 (26 Juli 2021 - 29 Agustus 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-1 (26 Juli 2021 - 29 Agustus 2021).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Web Dev\Web Kelas\Excel\Bulanan\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40F25DA-FD14-4C1E-8C13-3C8A89C9B9A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE10B18F-EFE7-4B80-9783-FF37F40A280E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:AG38"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -789,7 +789,7 @@
     <col min="31" max="33" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="18">
+    <row r="1" spans="1:33" ht="18" customHeight="1">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -838,7 +838,7 @@
       <c r="AF1" s="27"/>
       <c r="AG1" s="27"/>
     </row>
-    <row r="2" spans="1:33" ht="18">
+    <row r="2" spans="1:33" ht="18" customHeight="1">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="4" t="s">
@@ -935,7 +935,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="15.6">
+    <row r="3" spans="1:33" ht="15.6" customHeight="1">
       <c r="A3" s="26"/>
       <c r="B3" s="26"/>
       <c r="C3" s="8" t="s">
@@ -1032,7 +1032,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="15.6">
+    <row r="4" spans="1:33" ht="15.6" customHeight="1">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15.6">
+    <row r="5" spans="1:33" ht="15.6" customHeight="1">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="15.6">
+    <row r="6" spans="1:33" ht="15.6" customHeight="1">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="15.6">
+    <row r="7" spans="1:33" ht="15.6" customHeight="1">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="15.6">
+    <row r="8" spans="1:33" ht="15.6" customHeight="1">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="15.6">
+    <row r="9" spans="1:33" ht="15.6" customHeight="1">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1618,7 +1618,7 @@
       <c r="AF9" s="21"/>
       <c r="AG9" s="8"/>
     </row>
-    <row r="10" spans="1:33" ht="15.6">
+    <row r="10" spans="1:33" ht="15.6" customHeight="1">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="15.6">
+    <row r="11" spans="1:33" ht="15.6" customHeight="1">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1798,7 +1798,7 @@
       <c r="AF11" s="21"/>
       <c r="AG11" s="8"/>
     </row>
-    <row r="12" spans="1:33" ht="15.6">
+    <row r="12" spans="1:33" ht="15.6" customHeight="1">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="15.6">
+    <row r="13" spans="1:33" ht="15.6" customHeight="1">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AG13" s="8"/>
     </row>
-    <row r="14" spans="1:33" ht="15.6">
+    <row r="14" spans="1:33" ht="15.6" customHeight="1">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="15.6">
+    <row r="15" spans="1:33" ht="15.6" customHeight="1">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="15.6">
+    <row r="16" spans="1:33" ht="15.6" customHeight="1">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="15.6">
+    <row r="17" spans="1:33" ht="15.6" customHeight="1">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="15.6">
+    <row r="18" spans="1:33" ht="15.6" customHeight="1">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2481,7 +2481,7 @@
       <c r="AF18" s="21"/>
       <c r="AG18" s="8"/>
     </row>
-    <row r="19" spans="1:33" ht="15.6">
+    <row r="19" spans="1:33" ht="15.6" customHeight="1">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="15.6">
+    <row r="20" spans="1:33" ht="15.6" customHeight="1">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="15.6">
+    <row r="21" spans="1:33" ht="15.6" customHeight="1">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="15.6">
+    <row r="22" spans="1:33" ht="15.6" customHeight="1">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="15.6">
+    <row r="23" spans="1:33" ht="15.6" customHeight="1">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -2974,7 +2974,7 @@
       <c r="AF23" s="21"/>
       <c r="AG23" s="8"/>
     </row>
-    <row r="24" spans="1:33" ht="15.6">
+    <row r="24" spans="1:33" ht="15.6" customHeight="1">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="15.6">
+    <row r="25" spans="1:33" ht="15.6" customHeight="1">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="15.6">
+    <row r="26" spans="1:33" ht="15.6" customHeight="1">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="15.6">
+    <row r="27" spans="1:33" ht="15.6" customHeight="1">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="15.6">
+    <row r="28" spans="1:33" ht="15.6" customHeight="1">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="15.6">
+    <row r="29" spans="1:33" ht="15.6" customHeight="1">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="15.6">
+    <row r="30" spans="1:33" ht="15.6" customHeight="1">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -3631,7 +3631,7 @@
       <c r="AF30" s="21"/>
       <c r="AG30" s="8"/>
     </row>
-    <row r="31" spans="1:33" ht="15.6">
+    <row r="31" spans="1:33" ht="15.6" customHeight="1">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -3714,7 +3714,7 @@
       <c r="AF31" s="21"/>
       <c r="AG31" s="8"/>
     </row>
-    <row r="32" spans="1:33" ht="15.6">
+    <row r="32" spans="1:33" ht="15.6" customHeight="1">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="15.6">
+    <row r="33" spans="1:33" ht="15.6" customHeight="1">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="15.6">
+    <row r="34" spans="1:33" ht="15.6" customHeight="1">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="15.6">
+    <row r="35" spans="1:33" ht="15.6" customHeight="1">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="15.6">
+    <row r="36" spans="1:33" ht="15.6" customHeight="1">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="15.6">
+    <row r="37" spans="1:33" ht="15.6" customHeight="1">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="15.6">
+    <row r="38" spans="1:33" ht="15.6" customHeight="1">
       <c r="A38" s="2">
         <v>35</v>
       </c>

</xml_diff>